<commit_message>
added emailICS test cases - gruss; updated sprint 2 burn chart items and progress for tasks assigned to jgruss
</commit_message>
<xml_diff>
--- a/Documentation/backlogs/masterProductBacklog_4-17-16.xlsx
+++ b/Documentation/backlogs/masterProductBacklog_4-17-16.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="84">
   <si>
     <t>Sprints</t>
   </si>
@@ -260,6 +260,18 @@
   </si>
   <si>
     <t>Sprint 1 Backlog (Done)</t>
+  </si>
+  <si>
+    <t>Code compiles; waiting on SMTP IP</t>
+  </si>
+  <si>
+    <t>Class has most data</t>
+  </si>
+  <si>
+    <t>Anticipated, Waiting on SMPT IP</t>
+  </si>
+  <si>
+    <t>Anticipated, waiting on SMTP IP</t>
   </si>
 </sst>
 </file>
@@ -492,24 +504,24 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -856,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A29" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A43" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -877,11 +889,11 @@
       <c r="B1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
       <c r="F1" s="20" t="s">
         <v>34</v>
       </c>
@@ -891,14 +903,14 @@
       <c r="B2" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
-      <c r="B3" s="47"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="23" t="s">
         <v>24</v>
       </c>
@@ -910,7 +922,7 @@
     </row>
     <row r="4" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="47"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="22" t="s">
         <v>27</v>
       </c>
@@ -922,7 +934,7 @@
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
-      <c r="B5" s="47"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="22" t="s">
         <v>28</v>
       </c>
@@ -934,7 +946,7 @@
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20"/>
-      <c r="B6" s="47"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="22" t="s">
         <v>23</v>
       </c>
@@ -946,14 +958,14 @@
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="47"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="41" t="s">
         <v>78</v>
       </c>
       <c r="D7" s="24">
         <v>42477</v>
       </c>
-      <c r="E7" s="50"/>
+      <c r="E7" s="43"/>
     </row>
     <row r="8" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
@@ -996,8 +1008,8 @@
       <c r="E10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1015,10 +1027,10 @@
       <c r="E11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="44"/>
+      <c r="G11" s="50"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -1034,8 +1046,8 @@
         <v>42486</v>
       </c>
       <c r="E12" s="12"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1051,8 +1063,8 @@
         <v>42493</v>
       </c>
       <c r="E13" s="12"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -1060,8 +1072,8 @@
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
     </row>
     <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
@@ -1437,8 +1449,8 @@
       <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="48"/>
-      <c r="C41" s="49"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="48"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
     </row>
@@ -1588,10 +1600,12 @@
       <c r="D50" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E50" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F50" s="32"/>
+      <c r="E50" s="42">
+        <v>0.6</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
@@ -1609,7 +1623,9 @@
       <c r="E51" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F51" s="32"/>
+      <c r="F51" s="32" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
@@ -1627,7 +1643,9 @@
       <c r="E52" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F52" s="32"/>
+      <c r="F52" s="32" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
@@ -1643,7 +1661,7 @@
         <v>58</v>
       </c>
       <c r="E53" s="42">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="F53" s="32"/>
     </row>
@@ -1661,9 +1679,11 @@
         <v>58</v>
       </c>
       <c r="E54" s="42">
-        <v>0.5</v>
-      </c>
-      <c r="F54" s="32"/>
+        <v>0.6</v>
+      </c>
+      <c r="F54" s="32" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
@@ -1850,8 +1870,8 @@
       <c r="F69" s="13"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="48"/>
-      <c r="C70" s="49"/>
+      <c r="B70" s="47"/>
+      <c r="C70" s="48"/>
       <c r="F70" s="13"/>
       <c r="G70" s="13"/>
     </row>
@@ -1982,16 +2002,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="B70:C70"/>
     <mergeCell ref="B41:C41"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>